<commit_message>
added a script to compute the phycobillisome/chlorophyll a ratios and plot them as barplots with error bars
</commit_message>
<xml_diff>
--- a/WRITING/ToDo.xlsx
+++ b/WRITING/ToDo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\myr\home\ppalandre\Documents\scripts\Master-thesis\WRITING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB29719-3146-4F86-B434-AF83A3B6E8B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C10377C-E20E-4795-9128-BC9A8344733A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="To Do" sheetId="1" r:id="rId1"/>
+    <sheet name="Questions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Figures</t>
   </si>
@@ -82,13 +83,73 @@
   </si>
   <si>
     <t>Do all plots we are comparing together have the same scale?</t>
+  </si>
+  <si>
+    <t>Mat &amp; Met</t>
+  </si>
+  <si>
+    <t>Muss man Eisenammoniumcitrat als supplement angeben oder ist es Teil von BG11, wird aber später hinzugefügt?</t>
+  </si>
+  <si>
+    <t>Supplements</t>
+  </si>
+  <si>
+    <t>List of strains with antibiotica resistances</t>
+  </si>
+  <si>
+    <t>Cell culture and stains</t>
+  </si>
+  <si>
+    <t>Absorption measurements and data analysis (+ chlorophyll??)</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Pigment ratios</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
+    <t>AlphaFold</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>In depth analysis of DESeq2 dataset</t>
+  </si>
+  <si>
+    <t>Alle Kommazahlen mit .</t>
+  </si>
+  <si>
+    <t>Ist Rbp1-GFP auch mit pVZ322 plasmid und sfGFP?</t>
+  </si>
+  <si>
+    <t>Are there sources for WT and DualTag</t>
+  </si>
+  <si>
+    <t>Name of the spectrometer I used</t>
+  </si>
+  <si>
+    <t>Which publication to cite for BG11? Muss man ammonium ferric citrate extra nennen oder gehört es zum Rezept dazu?</t>
+  </si>
+  <si>
+    <t>Bei welchen Chemicals ist es wichtig, dass der Hersteller dabei steht und bei welchen nicht? Sonst ein "All Chemicals were purchased from Roth unless specified otherwhise" weil das bei den meisten der Fall ist?</t>
+  </si>
+  <si>
+    <t>Final version</t>
+  </si>
+  <si>
+    <t>Figure00_Vulcano plots von prot und RNA in introduction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +165,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,11 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,141 +504,280 @@
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A73622C-7CF9-4660-B013-78E85E4BDA08}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>